<commit_message>
Add functions for data set calling
</commit_message>
<xml_diff>
--- a/inst/extdata/expt_smry_cptac_cmbn.xlsx
+++ b/inst/extdata/expt_smry_cptac_cmbn.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Results\R\proteoQDA\data\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Results\R\proteoQDA\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -330,7 +330,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="125">
   <si>
     <t>Description</t>
   </si>
@@ -1402,7 +1402,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1579,12 +1579,6 @@
     </xf>
     <xf numFmtId="1" fontId="27" fillId="40" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="27" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="27" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1920,9 +1914,9 @@
   <dimension ref="A1:U61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="S1" sqref="S1"/>
-      <selection pane="bottomLeft" activeCell="F55" sqref="F55"/>
+      <selection pane="bottomLeft" activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1934,7 +1928,7 @@
     <col min="6" max="6" width="10.28515625" style="6" customWidth="1"/>
     <col min="7" max="7" width="19.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.140625" customWidth="1"/>
+    <col min="9" max="9" width="6.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="8.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.85546875" style="3" customWidth="1"/>
     <col min="13" max="13" width="6.42578125" style="3" customWidth="1"/>
@@ -2029,32 +2023,16 @@
       <c r="F2" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="G2" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="H2" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="I2" s="67">
-        <v>1</v>
-      </c>
+      <c r="G2" s="17"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
       <c r="J2" s="19"/>
-      <c r="K2" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="L2" s="20" t="s">
-        <v>122</v>
-      </c>
+      <c r="K2" s="19"/>
+      <c r="L2" s="20"/>
       <c r="M2" s="20"/>
-      <c r="N2" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="O2" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="P2" s="19" t="s">
-        <v>65</v>
-      </c>
+      <c r="N2" s="20"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
       <c r="Q2" s="17"/>
       <c r="R2" s="17"/>
       <c r="S2" s="21"/>
@@ -2080,7 +2058,7 @@
       <c r="H3" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="I3" s="67">
+      <c r="I3" s="23">
         <v>7</v>
       </c>
       <c r="J3" s="19"/>
@@ -2125,7 +2103,7 @@
       <c r="H4" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="I4" s="67">
+      <c r="I4" s="24">
         <v>1</v>
       </c>
       <c r="J4" s="24"/>
@@ -2170,7 +2148,7 @@
       <c r="H5" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="I5" s="67">
+      <c r="I5" s="24">
         <v>1</v>
       </c>
       <c r="J5" s="24"/>
@@ -2215,7 +2193,7 @@
       <c r="H6" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="I6" s="67">
+      <c r="I6" s="27">
         <v>7</v>
       </c>
       <c r="J6" s="24"/>
@@ -2260,7 +2238,7 @@
       <c r="H7" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="I7" s="68">
+      <c r="I7" s="24">
         <v>1</v>
       </c>
       <c r="J7" s="24"/>
@@ -2305,7 +2283,7 @@
       <c r="H8" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="I8" s="68">
+      <c r="I8" s="27">
         <v>7</v>
       </c>
       <c r="J8" s="24"/>
@@ -2350,7 +2328,7 @@
       <c r="H9" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="I9" s="68">
+      <c r="I9" s="27">
         <v>7</v>
       </c>
       <c r="J9" s="24"/>
@@ -2395,7 +2373,7 @@
       <c r="H10" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="I10" s="68">
+      <c r="I10" s="29">
         <v>1</v>
       </c>
       <c r="J10" s="29"/>
@@ -2440,7 +2418,7 @@
       <c r="H11" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="I11" s="68">
+      <c r="I11" s="32">
         <v>7</v>
       </c>
       <c r="J11" s="29"/>
@@ -2485,32 +2463,16 @@
       <c r="F12" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="G12" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="H12" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="I12" s="67">
-        <v>2</v>
-      </c>
+      <c r="G12" s="36"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
       <c r="J12" s="39"/>
-      <c r="K12" s="39" t="s">
-        <v>119</v>
-      </c>
-      <c r="L12" s="43" t="s">
-        <v>122</v>
-      </c>
+      <c r="K12" s="39"/>
+      <c r="L12" s="43"/>
       <c r="M12" s="39"/>
-      <c r="N12" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="O12" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="P12" s="39" t="s">
-        <v>65</v>
-      </c>
+      <c r="N12" s="39"/>
+      <c r="O12" s="38"/>
+      <c r="P12" s="39"/>
       <c r="Q12" s="36"/>
       <c r="R12" s="36"/>
       <c r="S12" s="40"/>
@@ -2536,7 +2498,7 @@
       <c r="H13" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="I13" s="67">
+      <c r="I13" s="42">
         <v>8</v>
       </c>
       <c r="J13" s="39"/>
@@ -2581,7 +2543,7 @@
       <c r="H14" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="I14" s="67">
+      <c r="I14" s="45">
         <v>2</v>
       </c>
       <c r="J14" s="46"/>
@@ -2626,7 +2588,7 @@
       <c r="H15" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="I15" s="67">
+      <c r="I15" s="45">
         <v>2</v>
       </c>
       <c r="J15" s="46"/>
@@ -2671,7 +2633,7 @@
       <c r="H16" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="I16" s="67">
+      <c r="I16" s="48">
         <v>8</v>
       </c>
       <c r="J16" s="46"/>
@@ -2716,7 +2678,7 @@
       <c r="H17" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="I17" s="68">
+      <c r="I17" s="45">
         <v>2</v>
       </c>
       <c r="J17" s="46"/>
@@ -2761,7 +2723,7 @@
       <c r="H18" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="I18" s="68">
+      <c r="I18" s="48">
         <v>8</v>
       </c>
       <c r="J18" s="46"/>
@@ -2806,7 +2768,7 @@
       <c r="H19" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="I19" s="68">
+      <c r="I19" s="48">
         <v>8</v>
       </c>
       <c r="J19" s="46"/>
@@ -2851,7 +2813,7 @@
       <c r="H20" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="I20" s="68">
+      <c r="I20" s="45">
         <v>2</v>
       </c>
       <c r="J20" s="46"/>
@@ -2896,7 +2858,7 @@
       <c r="H21" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="I21" s="68">
+      <c r="I21" s="48">
         <v>8</v>
       </c>
       <c r="J21" s="46"/>
@@ -2941,32 +2903,16 @@
       <c r="F22" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="G22" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="H22" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="I22" s="67">
-        <v>3</v>
-      </c>
+      <c r="G22" s="17"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
       <c r="J22" s="56"/>
-      <c r="K22" s="56" t="s">
-        <v>120</v>
-      </c>
-      <c r="L22" s="20" t="s">
-        <v>122</v>
-      </c>
+      <c r="K22" s="56"/>
+      <c r="L22" s="20"/>
       <c r="M22" s="20"/>
-      <c r="N22" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="O22" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="P22" s="19" t="s">
-        <v>95</v>
-      </c>
+      <c r="N22" s="20"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="19"/>
       <c r="Q22" s="17"/>
       <c r="R22" s="17"/>
       <c r="S22" s="21"/>
@@ -2992,7 +2938,7 @@
       <c r="H23" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="I23" s="67">
+      <c r="I23" s="23">
         <v>9</v>
       </c>
       <c r="J23" s="56"/>
@@ -3037,7 +2983,7 @@
       <c r="H24" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="I24" s="67">
+      <c r="I24" s="24">
         <v>3</v>
       </c>
       <c r="J24" s="57"/>
@@ -3082,7 +3028,7 @@
       <c r="H25" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="I25" s="67">
+      <c r="I25" s="24">
         <v>3</v>
       </c>
       <c r="J25" s="57"/>
@@ -3127,7 +3073,7 @@
       <c r="H26" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="I26" s="67">
+      <c r="I26" s="27">
         <v>9</v>
       </c>
       <c r="J26" s="57"/>
@@ -3172,7 +3118,7 @@
       <c r="H27" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="I27" s="68">
+      <c r="I27" s="24">
         <v>3</v>
       </c>
       <c r="J27" s="57"/>
@@ -3217,7 +3163,7 @@
       <c r="H28" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="I28" s="68">
+      <c r="I28" s="27">
         <v>9</v>
       </c>
       <c r="J28" s="57"/>
@@ -3262,7 +3208,7 @@
       <c r="H29" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="I29" s="68">
+      <c r="I29" s="27">
         <v>9</v>
       </c>
       <c r="J29" s="57"/>
@@ -3307,7 +3253,7 @@
       <c r="H30" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="I30" s="68">
+      <c r="I30" s="29">
         <v>3</v>
       </c>
       <c r="J30" s="58"/>
@@ -3352,7 +3298,7 @@
       <c r="H31" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="I31" s="68">
+      <c r="I31" s="32">
         <v>9</v>
       </c>
       <c r="J31" s="58"/>
@@ -3397,32 +3343,16 @@
       <c r="F32" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="G32" s="36" t="s">
-        <v>107</v>
-      </c>
-      <c r="H32" s="38" t="s">
-        <v>108</v>
-      </c>
-      <c r="I32" s="67">
-        <v>4</v>
-      </c>
+      <c r="G32" s="36"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="38"/>
       <c r="J32" s="38"/>
-      <c r="K32" s="38" t="s">
-        <v>120</v>
-      </c>
-      <c r="L32" s="43" t="s">
-        <v>122</v>
-      </c>
+      <c r="K32" s="38"/>
+      <c r="L32" s="43"/>
       <c r="M32" s="39"/>
-      <c r="N32" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="O32" s="38" t="s">
-        <v>108</v>
-      </c>
-      <c r="P32" s="39" t="s">
-        <v>95</v>
-      </c>
+      <c r="N32" s="39"/>
+      <c r="O32" s="38"/>
+      <c r="P32" s="39"/>
       <c r="Q32" s="36"/>
       <c r="R32" s="36"/>
       <c r="S32" s="40"/>
@@ -3448,7 +3378,7 @@
       <c r="H33" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="I33" s="67">
+      <c r="I33" s="42">
         <v>10</v>
       </c>
       <c r="J33" s="38"/>
@@ -3493,7 +3423,7 @@
       <c r="H34" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="I34" s="67">
+      <c r="I34" s="45">
         <v>4</v>
       </c>
       <c r="J34" s="45"/>
@@ -3538,7 +3468,7 @@
       <c r="H35" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="I35" s="67">
+      <c r="I35" s="45">
         <v>4</v>
       </c>
       <c r="J35" s="45"/>
@@ -3583,7 +3513,7 @@
       <c r="H36" s="48" t="s">
         <v>110</v>
       </c>
-      <c r="I36" s="67">
+      <c r="I36" s="48">
         <v>10</v>
       </c>
       <c r="J36" s="45"/>
@@ -3628,7 +3558,7 @@
       <c r="H37" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="I37" s="68">
+      <c r="I37" s="45">
         <v>4</v>
       </c>
       <c r="J37" s="45"/>
@@ -3673,7 +3603,7 @@
       <c r="H38" s="48" t="s">
         <v>110</v>
       </c>
-      <c r="I38" s="68">
+      <c r="I38" s="48">
         <v>10</v>
       </c>
       <c r="J38" s="45"/>
@@ -3718,7 +3648,7 @@
       <c r="H39" s="48" t="s">
         <v>110</v>
       </c>
-      <c r="I39" s="68">
+      <c r="I39" s="48">
         <v>10</v>
       </c>
       <c r="J39" s="45"/>
@@ -3763,7 +3693,7 @@
       <c r="H40" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="I40" s="68">
+      <c r="I40" s="45">
         <v>4</v>
       </c>
       <c r="J40" s="45"/>
@@ -3808,7 +3738,7 @@
       <c r="H41" s="48" t="s">
         <v>110</v>
       </c>
-      <c r="I41" s="68">
+      <c r="I41" s="48">
         <v>10</v>
       </c>
       <c r="J41" s="45"/>
@@ -3853,32 +3783,16 @@
       <c r="F42" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="G42" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="H42" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="I42" s="67">
-        <v>5</v>
-      </c>
+      <c r="G42" s="17"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
       <c r="J42" s="59"/>
-      <c r="K42" s="59" t="s">
-        <v>121</v>
-      </c>
-      <c r="L42" s="20" t="s">
-        <v>122</v>
-      </c>
+      <c r="K42" s="59"/>
+      <c r="L42" s="20"/>
       <c r="M42" s="20"/>
-      <c r="N42" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="O42" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="P42" s="19" t="s">
-        <v>69</v>
-      </c>
+      <c r="N42" s="20"/>
+      <c r="O42" s="19"/>
+      <c r="P42" s="19"/>
       <c r="Q42" s="17"/>
       <c r="R42" s="17"/>
       <c r="S42" s="21"/>
@@ -3904,7 +3818,7 @@
       <c r="H43" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="I43" s="67">
+      <c r="I43" s="23">
         <v>11</v>
       </c>
       <c r="J43" s="59"/>
@@ -3949,7 +3863,7 @@
       <c r="H44" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="I44" s="67">
+      <c r="I44" s="24">
         <v>5</v>
       </c>
       <c r="J44" s="60"/>
@@ -3994,7 +3908,7 @@
       <c r="H45" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="I45" s="67">
+      <c r="I45" s="24">
         <v>5</v>
       </c>
       <c r="J45" s="60"/>
@@ -4039,7 +3953,7 @@
       <c r="H46" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="I46" s="67">
+      <c r="I46" s="27">
         <v>11</v>
       </c>
       <c r="J46" s="60"/>
@@ -4084,7 +3998,7 @@
       <c r="H47" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="I47" s="68">
+      <c r="I47" s="24">
         <v>5</v>
       </c>
       <c r="J47" s="60"/>
@@ -4129,7 +4043,7 @@
       <c r="H48" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="I48" s="68">
+      <c r="I48" s="27">
         <v>11</v>
       </c>
       <c r="J48" s="60"/>
@@ -4174,7 +4088,7 @@
       <c r="H49" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="I49" s="68">
+      <c r="I49" s="27">
         <v>11</v>
       </c>
       <c r="J49" s="60"/>
@@ -4219,7 +4133,7 @@
       <c r="H50" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="I50" s="68">
+      <c r="I50" s="29">
         <v>5</v>
       </c>
       <c r="J50" s="61"/>
@@ -4264,7 +4178,7 @@
       <c r="H51" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="I51" s="68">
+      <c r="I51" s="32">
         <v>11</v>
       </c>
       <c r="J51" s="61"/>
@@ -4309,32 +4223,16 @@
       <c r="F52" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="G52" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="H52" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="I52" s="67">
-        <v>6</v>
-      </c>
+      <c r="G52" s="36"/>
+      <c r="H52" s="38"/>
+      <c r="I52" s="38"/>
       <c r="J52" s="62"/>
-      <c r="K52" s="62" t="s">
-        <v>121</v>
-      </c>
-      <c r="L52" s="43" t="s">
-        <v>122</v>
-      </c>
+      <c r="K52" s="62"/>
+      <c r="L52" s="43"/>
       <c r="M52" s="39"/>
-      <c r="N52" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="O52" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="P52" s="39" t="s">
-        <v>69</v>
-      </c>
+      <c r="N52" s="39"/>
+      <c r="O52" s="38"/>
+      <c r="P52" s="39"/>
       <c r="Q52" s="36"/>
       <c r="R52" s="36"/>
       <c r="S52" s="40"/>
@@ -4360,7 +4258,7 @@
       <c r="H53" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="I53" s="67">
+      <c r="I53" s="42">
         <v>12</v>
       </c>
       <c r="J53" s="62"/>
@@ -4405,7 +4303,7 @@
       <c r="H54" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="I54" s="67">
+      <c r="I54" s="45">
         <v>6</v>
       </c>
       <c r="J54" s="63"/>
@@ -4450,7 +4348,7 @@
       <c r="H55" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="I55" s="67">
+      <c r="I55" s="45">
         <v>6</v>
       </c>
       <c r="J55" s="63"/>
@@ -4495,7 +4393,7 @@
       <c r="H56" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="I56" s="67">
+      <c r="I56" s="48">
         <v>12</v>
       </c>
       <c r="J56" s="63"/>
@@ -4540,7 +4438,7 @@
       <c r="H57" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="I57" s="68">
+      <c r="I57" s="45">
         <v>6</v>
       </c>
       <c r="J57" s="63"/>
@@ -4585,7 +4483,7 @@
       <c r="H58" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="I58" s="68">
+      <c r="I58" s="48">
         <v>12</v>
       </c>
       <c r="J58" s="63"/>
@@ -4630,7 +4528,7 @@
       <c r="H59" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="I59" s="68">
+      <c r="I59" s="48">
         <v>12</v>
       </c>
       <c r="J59" s="63"/>
@@ -4675,7 +4573,7 @@
       <c r="H60" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="I60" s="68">
+      <c r="I60" s="45">
         <v>6</v>
       </c>
       <c r="J60" s="63"/>
@@ -4720,7 +4618,7 @@
       <c r="H61" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="I61" s="68">
+      <c r="I61" s="48">
         <v>12</v>
       </c>
       <c r="J61" s="63"/>

</xml_diff>

<commit_message>
Update calling functions to data sets
</commit_message>
<xml_diff>
--- a/inst/extdata/expt_smry_cptac_cmbn.xlsx
+++ b/inst/extdata/expt_smry_cptac_cmbn.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Params" sheetId="13" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Setup!$B$1:$U$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Setup!$B$1:$X$61</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -177,11 +177,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>Samples will be included in analysis</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>Optional: a priori knowledge of sample groups</t>
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -194,7 +207,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -245,7 +258,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
+    <comment ref="R1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -259,7 +272,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0">
+    <comment ref="S1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -273,7 +286,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0">
+    <comment ref="T1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -286,7 +299,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0">
+    <comment ref="U1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -299,7 +312,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0" shapeId="0">
+    <comment ref="V1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -312,7 +325,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0" shapeId="0">
+    <comment ref="W1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -330,7 +343,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="125">
   <si>
     <t>Description</t>
   </si>
@@ -1911,12 +1924,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U61"/>
+  <dimension ref="A1:X61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="S1" sqref="S1"/>
-      <selection pane="bottomLeft" activeCell="U5" sqref="U5"/>
+      <selection pane="bottomLeft" activeCell="J42" sqref="J42:J61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1926,22 +1939,23 @@
     <col min="3" max="4" width="9.140625" style="2"/>
     <col min="5" max="5" width="9.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.28515625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="8.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.85546875" style="3" customWidth="1"/>
-    <col min="13" max="13" width="6.42578125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="6.140625" style="7" customWidth="1"/>
-    <col min="15" max="15" width="10.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="9.140625" style="8" customWidth="1"/>
-    <col min="18" max="18" width="10.5703125" style="5" customWidth="1"/>
-    <col min="19" max="19" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9" style="1" customWidth="1"/>
-    <col min="21" max="21" width="24" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="19.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="19.5703125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="8.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.85546875" style="3" customWidth="1"/>
+    <col min="16" max="16" width="6.42578125" style="3" customWidth="1"/>
+    <col min="17" max="17" width="6.140625" style="7" customWidth="1"/>
+    <col min="18" max="18" width="10.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="9.140625" style="8" customWidth="1"/>
+    <col min="21" max="21" width="10.5703125" style="5" customWidth="1"/>
+    <col min="22" max="22" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9" style="1" customWidth="1"/>
+    <col min="24" max="24" width="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>6</v>
       </c>
@@ -1963,50 +1977,59 @@
       <c r="G1" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="53" t="s">
+      <c r="H1" s="50" t="s">
+        <v>119</v>
+      </c>
+      <c r="I1" s="50" t="s">
+        <v>120</v>
+      </c>
+      <c r="J1" s="50" t="s">
+        <v>121</v>
+      </c>
+      <c r="K1" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="66" t="s">
+      <c r="L1" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="M1" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="N1" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="O1" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="P1" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="Q1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="13" t="s">
+      <c r="R1" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="S1" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="Q1" s="54" t="s">
+      <c r="T1" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="55" t="s">
+      <c r="U1" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="S1" s="51" t="s">
+      <c r="V1" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="T1" s="51" t="s">
+      <c r="W1" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="U1" s="52" t="s">
+      <c r="X1" s="52" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>41</v>
       </c>
@@ -2024,24 +2047,27 @@
         <v>124</v>
       </c>
       <c r="G2" s="17"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
       <c r="K2" s="19"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
-      <c r="S2" s="21"/>
-      <c r="T2" s="22"/>
-      <c r="U2" s="14" t="s">
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="17"/>
+      <c r="U2" s="17"/>
+      <c r="V2" s="21"/>
+      <c r="W2" s="22"/>
+      <c r="X2" s="14" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>51</v>
       </c>
@@ -2051,42 +2077,31 @@
       <c r="C3" s="15"/>
       <c r="D3" s="15"/>
       <c r="E3" s="16"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="H3" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="I3" s="23">
-        <v>7</v>
-      </c>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="L3" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="O3" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="P3" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="21"/>
-      <c r="T3" s="22"/>
-      <c r="U3" s="14" t="s">
+      <c r="F3" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="17"/>
+      <c r="U3" s="17"/>
+      <c r="V3" s="21"/>
+      <c r="W3" s="22"/>
+      <c r="X3" s="14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>42</v>
       </c>
@@ -2100,38 +2115,43 @@
       <c r="G4" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="I4" s="24">
+      <c r="L4" s="24">
         <v>1</v>
       </c>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24" t="s">
+      <c r="M4" s="24"/>
+      <c r="N4" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="O4" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25" t="s">
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="R4" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="P4" s="24" t="s">
+      <c r="S4" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="26"/>
-      <c r="T4" s="22"/>
-      <c r="U4" s="14" t="s">
+      <c r="T4" s="14"/>
+      <c r="U4" s="14"/>
+      <c r="V4" s="26"/>
+      <c r="W4" s="22"/>
+      <c r="X4" s="14" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>43</v>
       </c>
@@ -2145,38 +2165,43 @@
       <c r="G5" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="24" t="s">
+      <c r="H5" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="I5" s="24">
+      <c r="L5" s="24">
         <v>1</v>
       </c>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24" t="s">
+      <c r="M5" s="24"/>
+      <c r="N5" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="L5" s="25" t="s">
+      <c r="O5" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25" t="s">
+      <c r="P5" s="25"/>
+      <c r="Q5" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="O5" s="24" t="s">
+      <c r="R5" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="P5" s="24" t="s">
+      <c r="S5" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="26"/>
-      <c r="T5" s="22"/>
-      <c r="U5" s="14" t="s">
+      <c r="T5" s="14"/>
+      <c r="U5" s="14"/>
+      <c r="V5" s="26"/>
+      <c r="W5" s="22"/>
+      <c r="X5" s="14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>52</v>
       </c>
@@ -2190,38 +2215,43 @@
       <c r="G6" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="H6" s="27" t="s">
+      <c r="H6" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="I6" s="27">
+      <c r="L6" s="27">
         <v>7</v>
       </c>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24" t="s">
+      <c r="M6" s="24"/>
+      <c r="N6" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="L6" s="27" t="s">
+      <c r="O6" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="M6" s="25"/>
-      <c r="N6" s="25" t="s">
+      <c r="P6" s="25"/>
+      <c r="Q6" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="O6" s="27" t="s">
+      <c r="R6" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="P6" s="25" t="s">
+      <c r="S6" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14"/>
-      <c r="S6" s="26"/>
-      <c r="T6" s="22"/>
-      <c r="U6" s="14" t="s">
+      <c r="T6" s="14"/>
+      <c r="U6" s="14"/>
+      <c r="V6" s="26"/>
+      <c r="W6" s="22"/>
+      <c r="X6" s="14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>44</v>
       </c>
@@ -2235,38 +2265,43 @@
       <c r="G7" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="H7" s="24" t="s">
+      <c r="H7" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="I7" s="24">
+      <c r="L7" s="24">
         <v>1</v>
       </c>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24" t="s">
+      <c r="M7" s="24"/>
+      <c r="N7" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="L7" s="25" t="s">
+      <c r="O7" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25" t="s">
+      <c r="P7" s="25"/>
+      <c r="Q7" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="O7" s="24" t="s">
+      <c r="R7" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="P7" s="24" t="s">
+      <c r="S7" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="26"/>
-      <c r="T7" s="22"/>
-      <c r="U7" s="14" t="s">
+      <c r="T7" s="14"/>
+      <c r="U7" s="14"/>
+      <c r="V7" s="26"/>
+      <c r="W7" s="22"/>
+      <c r="X7" s="14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>53</v>
       </c>
@@ -2280,38 +2315,43 @@
       <c r="G8" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="27" t="s">
+      <c r="H8" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="I8" s="27">
+      <c r="L8" s="27">
         <v>7</v>
       </c>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24" t="s">
+      <c r="M8" s="24"/>
+      <c r="N8" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="L8" s="27" t="s">
+      <c r="O8" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25" t="s">
+      <c r="P8" s="25"/>
+      <c r="Q8" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="O8" s="27" t="s">
+      <c r="R8" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="P8" s="25" t="s">
+      <c r="S8" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="26"/>
-      <c r="T8" s="22"/>
-      <c r="U8" s="14" t="s">
+      <c r="T8" s="14"/>
+      <c r="U8" s="14"/>
+      <c r="V8" s="26"/>
+      <c r="W8" s="22"/>
+      <c r="X8" s="14" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>54</v>
       </c>
@@ -2325,38 +2365,43 @@
       <c r="G9" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="27" t="s">
+      <c r="H9" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="I9" s="27">
+      <c r="L9" s="27">
         <v>7</v>
       </c>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24" t="s">
+      <c r="M9" s="24"/>
+      <c r="N9" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="L9" s="27" t="s">
+      <c r="O9" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="M9" s="25"/>
-      <c r="N9" s="25" t="s">
+      <c r="P9" s="25"/>
+      <c r="Q9" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="O9" s="27" t="s">
+      <c r="R9" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="P9" s="25" t="s">
+      <c r="S9" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="14"/>
-      <c r="S9" s="26"/>
-      <c r="T9" s="22"/>
-      <c r="U9" s="14" t="s">
+      <c r="T9" s="14"/>
+      <c r="U9" s="14"/>
+      <c r="V9" s="26"/>
+      <c r="W9" s="22"/>
+      <c r="X9" s="14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
         <v>45</v>
       </c>
@@ -2370,38 +2415,43 @@
       <c r="G10" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="H10" s="29" t="s">
+      <c r="H10" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="I10" s="29">
+      <c r="L10" s="29">
         <v>1</v>
       </c>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29" t="s">
+      <c r="M10" s="29"/>
+      <c r="N10" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="L10" s="30" t="s">
+      <c r="O10" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="M10" s="30"/>
-      <c r="N10" s="30" t="s">
+      <c r="P10" s="30"/>
+      <c r="Q10" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="O10" s="29" t="s">
+      <c r="R10" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="P10" s="29" t="s">
+      <c r="S10" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="Q10" s="28"/>
-      <c r="R10" s="28"/>
-      <c r="S10" s="31"/>
-      <c r="T10" s="22"/>
-      <c r="U10" s="14" t="s">
+      <c r="T10" s="28"/>
+      <c r="U10" s="28"/>
+      <c r="V10" s="31"/>
+      <c r="W10" s="22"/>
+      <c r="X10" s="14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
         <v>55</v>
       </c>
@@ -2415,38 +2465,43 @@
       <c r="G11" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="H11" s="32" t="s">
+      <c r="H11" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="I11" s="32">
+      <c r="L11" s="32">
         <v>7</v>
       </c>
-      <c r="J11" s="29"/>
-      <c r="K11" s="29" t="s">
+      <c r="M11" s="29"/>
+      <c r="N11" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="L11" s="32" t="s">
+      <c r="O11" s="32" t="s">
         <v>123</v>
       </c>
-      <c r="M11" s="30"/>
-      <c r="N11" s="30" t="s">
+      <c r="P11" s="30"/>
+      <c r="Q11" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="O11" s="32" t="s">
+      <c r="R11" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="P11" s="30" t="s">
+      <c r="S11" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="Q11" s="28"/>
-      <c r="R11" s="28"/>
-      <c r="S11" s="31"/>
-      <c r="T11" s="22"/>
-      <c r="U11" s="14" t="s">
+      <c r="T11" s="28"/>
+      <c r="U11" s="28"/>
+      <c r="V11" s="31"/>
+      <c r="W11" s="22"/>
+      <c r="X11" s="14" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36" t="s">
         <v>46</v>
       </c>
@@ -2464,24 +2519,27 @@
         <v>124</v>
       </c>
       <c r="G12" s="36"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="43"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="38"/>
       <c r="M12" s="39"/>
       <c r="N12" s="39"/>
-      <c r="O12" s="38"/>
+      <c r="O12" s="43"/>
       <c r="P12" s="39"/>
-      <c r="Q12" s="36"/>
-      <c r="R12" s="36"/>
-      <c r="S12" s="40"/>
-      <c r="T12" s="41"/>
-      <c r="U12" s="33" t="s">
+      <c r="Q12" s="39"/>
+      <c r="R12" s="38"/>
+      <c r="S12" s="39"/>
+      <c r="T12" s="36"/>
+      <c r="U12" s="36"/>
+      <c r="V12" s="40"/>
+      <c r="W12" s="41"/>
+      <c r="X12" s="33" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="36" t="s">
         <v>56</v>
       </c>
@@ -2491,42 +2549,31 @@
       <c r="C13" s="34"/>
       <c r="D13" s="34"/>
       <c r="E13" s="35"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="H13" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="I13" s="42">
-        <v>8</v>
-      </c>
-      <c r="J13" s="39"/>
-      <c r="K13" s="39" t="s">
-        <v>119</v>
-      </c>
-      <c r="L13" s="64" t="s">
-        <v>123</v>
-      </c>
+      <c r="F13" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="42"/>
       <c r="M13" s="39"/>
-      <c r="N13" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="O13" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="P13" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q13" s="36"/>
-      <c r="R13" s="36"/>
-      <c r="S13" s="40"/>
-      <c r="T13" s="41"/>
-      <c r="U13" s="33" t="s">
+      <c r="N13" s="39"/>
+      <c r="O13" s="64"/>
+      <c r="P13" s="39"/>
+      <c r="Q13" s="39"/>
+      <c r="R13" s="42"/>
+      <c r="S13" s="43"/>
+      <c r="T13" s="36"/>
+      <c r="U13" s="36"/>
+      <c r="V13" s="40"/>
+      <c r="W13" s="41"/>
+      <c r="X13" s="33" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="44" t="s">
         <v>47</v>
       </c>
@@ -2540,38 +2587,43 @@
       <c r="G14" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="H14" s="45" t="s">
+      <c r="H14" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="I14" s="44"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="I14" s="45">
+      <c r="L14" s="45">
         <v>2</v>
-      </c>
-      <c r="J14" s="46"/>
-      <c r="K14" s="46" t="s">
-        <v>119</v>
-      </c>
-      <c r="L14" s="49" t="s">
-        <v>122</v>
       </c>
       <c r="M14" s="46"/>
       <c r="N14" s="46" t="s">
+        <v>119</v>
+      </c>
+      <c r="O14" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="P14" s="46"/>
+      <c r="Q14" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="O14" s="45" t="s">
+      <c r="R14" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="P14" s="46" t="s">
+      <c r="S14" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="Q14" s="44"/>
-      <c r="R14" s="44"/>
-      <c r="S14" s="47"/>
-      <c r="T14" s="41"/>
-      <c r="U14" s="33" t="s">
+      <c r="T14" s="44"/>
+      <c r="U14" s="44"/>
+      <c r="V14" s="47"/>
+      <c r="W14" s="41"/>
+      <c r="X14" s="33" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="44" t="s">
         <v>48</v>
       </c>
@@ -2585,38 +2637,43 @@
       <c r="G15" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="H15" s="45" t="s">
+      <c r="H15" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="I15" s="44"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="I15" s="45">
+      <c r="L15" s="45">
         <v>2</v>
-      </c>
-      <c r="J15" s="46"/>
-      <c r="K15" s="46" t="s">
-        <v>119</v>
-      </c>
-      <c r="L15" s="49" t="s">
-        <v>122</v>
       </c>
       <c r="M15" s="46"/>
       <c r="N15" s="46" t="s">
+        <v>119</v>
+      </c>
+      <c r="O15" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="P15" s="46"/>
+      <c r="Q15" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="O15" s="45" t="s">
+      <c r="R15" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="P15" s="46" t="s">
+      <c r="S15" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="Q15" s="44"/>
-      <c r="R15" s="44"/>
-      <c r="S15" s="47"/>
-      <c r="T15" s="41"/>
-      <c r="U15" s="33" t="s">
+      <c r="T15" s="44"/>
+      <c r="U15" s="44"/>
+      <c r="V15" s="47"/>
+      <c r="W15" s="41"/>
+      <c r="X15" s="33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="44" t="s">
         <v>57</v>
       </c>
@@ -2630,38 +2687,43 @@
       <c r="G16" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="H16" s="48" t="s">
+      <c r="H16" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="I16" s="44"/>
+      <c r="J16" s="44"/>
+      <c r="K16" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="I16" s="48">
+      <c r="L16" s="48">
         <v>8</v>
-      </c>
-      <c r="J16" s="46"/>
-      <c r="K16" s="46" t="s">
-        <v>119</v>
-      </c>
-      <c r="L16" s="65" t="s">
-        <v>123</v>
       </c>
       <c r="M16" s="46"/>
       <c r="N16" s="46" t="s">
+        <v>119</v>
+      </c>
+      <c r="O16" s="65" t="s">
+        <v>123</v>
+      </c>
+      <c r="P16" s="46"/>
+      <c r="Q16" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="O16" s="48" t="s">
+      <c r="R16" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="P16" s="49" t="s">
+      <c r="S16" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="Q16" s="44"/>
-      <c r="R16" s="44"/>
-      <c r="S16" s="47"/>
-      <c r="T16" s="41"/>
-      <c r="U16" s="33" t="s">
+      <c r="T16" s="44"/>
+      <c r="U16" s="44"/>
+      <c r="V16" s="47"/>
+      <c r="W16" s="41"/>
+      <c r="X16" s="33" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="44" t="s">
         <v>49</v>
       </c>
@@ -2675,38 +2737,43 @@
       <c r="G17" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="H17" s="45" t="s">
+      <c r="H17" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="I17" s="44"/>
+      <c r="J17" s="44"/>
+      <c r="K17" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="I17" s="45">
+      <c r="L17" s="45">
         <v>2</v>
-      </c>
-      <c r="J17" s="46"/>
-      <c r="K17" s="46" t="s">
-        <v>119</v>
-      </c>
-      <c r="L17" s="49" t="s">
-        <v>122</v>
       </c>
       <c r="M17" s="46"/>
       <c r="N17" s="46" t="s">
+        <v>119</v>
+      </c>
+      <c r="O17" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="P17" s="46"/>
+      <c r="Q17" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="O17" s="45" t="s">
+      <c r="R17" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="P17" s="46" t="s">
+      <c r="S17" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="Q17" s="44"/>
-      <c r="R17" s="44"/>
-      <c r="S17" s="47"/>
-      <c r="T17" s="41"/>
-      <c r="U17" s="33" t="s">
+      <c r="T17" s="44"/>
+      <c r="U17" s="44"/>
+      <c r="V17" s="47"/>
+      <c r="W17" s="41"/>
+      <c r="X17" s="33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="44" t="s">
         <v>58</v>
       </c>
@@ -2720,38 +2787,43 @@
       <c r="G18" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="H18" s="48" t="s">
+      <c r="H18" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="I18" s="44"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="I18" s="48">
+      <c r="L18" s="48">
         <v>8</v>
-      </c>
-      <c r="J18" s="46"/>
-      <c r="K18" s="46" t="s">
-        <v>119</v>
-      </c>
-      <c r="L18" s="65" t="s">
-        <v>123</v>
       </c>
       <c r="M18" s="46"/>
       <c r="N18" s="46" t="s">
+        <v>119</v>
+      </c>
+      <c r="O18" s="65" t="s">
+        <v>123</v>
+      </c>
+      <c r="P18" s="46"/>
+      <c r="Q18" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="O18" s="48" t="s">
+      <c r="R18" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="P18" s="49" t="s">
+      <c r="S18" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="Q18" s="44"/>
-      <c r="R18" s="44"/>
-      <c r="S18" s="47"/>
-      <c r="T18" s="41"/>
-      <c r="U18" s="33" t="s">
+      <c r="T18" s="44"/>
+      <c r="U18" s="44"/>
+      <c r="V18" s="47"/>
+      <c r="W18" s="41"/>
+      <c r="X18" s="33" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="44" t="s">
         <v>59</v>
       </c>
@@ -2765,38 +2837,43 @@
       <c r="G19" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="H19" s="48" t="s">
+      <c r="H19" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
+      <c r="K19" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="I19" s="48">
+      <c r="L19" s="48">
         <v>8</v>
-      </c>
-      <c r="J19" s="46"/>
-      <c r="K19" s="46" t="s">
-        <v>119</v>
-      </c>
-      <c r="L19" s="65" t="s">
-        <v>123</v>
       </c>
       <c r="M19" s="46"/>
       <c r="N19" s="46" t="s">
+        <v>119</v>
+      </c>
+      <c r="O19" s="65" t="s">
+        <v>123</v>
+      </c>
+      <c r="P19" s="46"/>
+      <c r="Q19" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="O19" s="48" t="s">
+      <c r="R19" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="P19" s="49" t="s">
+      <c r="S19" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="Q19" s="44"/>
-      <c r="R19" s="44"/>
-      <c r="S19" s="47"/>
-      <c r="T19" s="41"/>
-      <c r="U19" s="33" t="s">
+      <c r="T19" s="44"/>
+      <c r="U19" s="44"/>
+      <c r="V19" s="47"/>
+      <c r="W19" s="41"/>
+      <c r="X19" s="33" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="44" t="s">
         <v>50</v>
       </c>
@@ -2810,38 +2887,43 @@
       <c r="G20" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="H20" s="45" t="s">
+      <c r="H20" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
+      <c r="K20" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="I20" s="45">
+      <c r="L20" s="45">
         <v>2</v>
-      </c>
-      <c r="J20" s="46"/>
-      <c r="K20" s="46" t="s">
-        <v>119</v>
-      </c>
-      <c r="L20" s="49" t="s">
-        <v>122</v>
       </c>
       <c r="M20" s="46"/>
       <c r="N20" s="46" t="s">
+        <v>119</v>
+      </c>
+      <c r="O20" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="P20" s="46"/>
+      <c r="Q20" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="O20" s="45" t="s">
+      <c r="R20" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="P20" s="46" t="s">
+      <c r="S20" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="Q20" s="44"/>
-      <c r="R20" s="44"/>
-      <c r="S20" s="47"/>
-      <c r="T20" s="41"/>
-      <c r="U20" s="33" t="s">
+      <c r="T20" s="44"/>
+      <c r="U20" s="44"/>
+      <c r="V20" s="47"/>
+      <c r="W20" s="41"/>
+      <c r="X20" s="33" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="44" t="s">
         <v>60</v>
       </c>
@@ -2855,38 +2937,43 @@
       <c r="G21" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="H21" s="48" t="s">
+      <c r="H21" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="I21" s="44"/>
+      <c r="J21" s="44"/>
+      <c r="K21" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="I21" s="48">
+      <c r="L21" s="48">
         <v>8</v>
-      </c>
-      <c r="J21" s="46"/>
-      <c r="K21" s="46" t="s">
-        <v>119</v>
-      </c>
-      <c r="L21" s="65" t="s">
-        <v>123</v>
       </c>
       <c r="M21" s="46"/>
       <c r="N21" s="46" t="s">
+        <v>119</v>
+      </c>
+      <c r="O21" s="65" t="s">
+        <v>123</v>
+      </c>
+      <c r="P21" s="46"/>
+      <c r="Q21" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="O21" s="48" t="s">
+      <c r="R21" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="P21" s="49" t="s">
+      <c r="S21" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="Q21" s="44"/>
-      <c r="R21" s="44"/>
-      <c r="S21" s="47"/>
-      <c r="T21" s="41"/>
-      <c r="U21" s="33" t="s">
+      <c r="T21" s="44"/>
+      <c r="U21" s="44"/>
+      <c r="V21" s="47"/>
+      <c r="W21" s="41"/>
+      <c r="X21" s="33" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
         <v>93</v>
       </c>
@@ -2904,24 +2991,27 @@
         <v>124</v>
       </c>
       <c r="G22" s="17"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19"/>
-      <c r="J22" s="56"/>
-      <c r="K22" s="56"/>
-      <c r="L22" s="20"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="20"/>
-      <c r="O22" s="19"/>
-      <c r="P22" s="19"/>
-      <c r="Q22" s="17"/>
-      <c r="R22" s="17"/>
-      <c r="S22" s="21"/>
-      <c r="T22" s="22"/>
-      <c r="U22" s="14" t="s">
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="56"/>
+      <c r="N22" s="56"/>
+      <c r="O22" s="20"/>
+      <c r="P22" s="20"/>
+      <c r="Q22" s="20"/>
+      <c r="R22" s="19"/>
+      <c r="S22" s="19"/>
+      <c r="T22" s="17"/>
+      <c r="U22" s="17"/>
+      <c r="V22" s="21"/>
+      <c r="W22" s="22"/>
+      <c r="X22" s="14" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>96</v>
       </c>
@@ -2931,42 +3021,31 @@
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
       <c r="E23" s="16"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="H23" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="I23" s="23">
-        <v>9</v>
-      </c>
-      <c r="J23" s="56"/>
-      <c r="K23" s="56" t="s">
-        <v>120</v>
-      </c>
-      <c r="L23" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="M23" s="20"/>
-      <c r="N23" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="O23" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="P23" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q23" s="17"/>
-      <c r="R23" s="17"/>
-      <c r="S23" s="21"/>
-      <c r="T23" s="22"/>
-      <c r="U23" s="14" t="s">
+      <c r="F23" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="56"/>
+      <c r="N23" s="56"/>
+      <c r="O23" s="23"/>
+      <c r="P23" s="20"/>
+      <c r="Q23" s="20"/>
+      <c r="R23" s="23"/>
+      <c r="S23" s="20"/>
+      <c r="T23" s="17"/>
+      <c r="U23" s="17"/>
+      <c r="V23" s="21"/>
+      <c r="W23" s="22"/>
+      <c r="X23" s="14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>99</v>
       </c>
@@ -2980,38 +3059,43 @@
       <c r="G24" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="H24" s="24" t="s">
+      <c r="H24" s="14"/>
+      <c r="I24" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="J24" s="14"/>
+      <c r="K24" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="I24" s="24">
+      <c r="L24" s="24">
         <v>3</v>
       </c>
-      <c r="J24" s="57"/>
-      <c r="K24" s="57" t="s">
+      <c r="M24" s="57"/>
+      <c r="N24" s="57" t="s">
         <v>120</v>
       </c>
-      <c r="L24" s="25" t="s">
+      <c r="O24" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="M24" s="25"/>
-      <c r="N24" s="25" t="s">
+      <c r="P24" s="25"/>
+      <c r="Q24" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="O24" s="24" t="s">
+      <c r="R24" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="P24" s="24" t="s">
+      <c r="S24" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="Q24" s="14"/>
-      <c r="R24" s="14"/>
-      <c r="S24" s="26"/>
-      <c r="T24" s="22"/>
-      <c r="U24" s="14" t="s">
+      <c r="T24" s="14"/>
+      <c r="U24" s="14"/>
+      <c r="V24" s="26"/>
+      <c r="W24" s="22"/>
+      <c r="X24" s="14" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>100</v>
       </c>
@@ -3025,38 +3109,43 @@
       <c r="G25" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="H25" s="24" t="s">
+      <c r="H25" s="14"/>
+      <c r="I25" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="J25" s="14"/>
+      <c r="K25" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="I25" s="24">
+      <c r="L25" s="24">
         <v>3</v>
       </c>
-      <c r="J25" s="57"/>
-      <c r="K25" s="57" t="s">
+      <c r="M25" s="57"/>
+      <c r="N25" s="57" t="s">
         <v>120</v>
       </c>
-      <c r="L25" s="25" t="s">
+      <c r="O25" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="M25" s="25"/>
-      <c r="N25" s="25" t="s">
+      <c r="P25" s="25"/>
+      <c r="Q25" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="O25" s="24" t="s">
+      <c r="R25" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="P25" s="24" t="s">
+      <c r="S25" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="Q25" s="14"/>
-      <c r="R25" s="14"/>
-      <c r="S25" s="26"/>
-      <c r="T25" s="22"/>
-      <c r="U25" s="14" t="s">
+      <c r="T25" s="14"/>
+      <c r="U25" s="14"/>
+      <c r="V25" s="26"/>
+      <c r="W25" s="22"/>
+      <c r="X25" s="14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
         <v>101</v>
       </c>
@@ -3070,38 +3159,43 @@
       <c r="G26" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="H26" s="27" t="s">
+      <c r="H26" s="14"/>
+      <c r="I26" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="J26" s="14"/>
+      <c r="K26" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="I26" s="27">
+      <c r="L26" s="27">
         <v>9</v>
       </c>
-      <c r="J26" s="57"/>
-      <c r="K26" s="57" t="s">
+      <c r="M26" s="57"/>
+      <c r="N26" s="57" t="s">
         <v>120</v>
       </c>
-      <c r="L26" s="27" t="s">
+      <c r="O26" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="M26" s="25"/>
-      <c r="N26" s="25" t="s">
+      <c r="P26" s="25"/>
+      <c r="Q26" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="O26" s="27" t="s">
+      <c r="R26" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="P26" s="25" t="s">
+      <c r="S26" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="Q26" s="14"/>
-      <c r="R26" s="14"/>
-      <c r="S26" s="26"/>
-      <c r="T26" s="22"/>
-      <c r="U26" s="14" t="s">
+      <c r="T26" s="14"/>
+      <c r="U26" s="14"/>
+      <c r="V26" s="26"/>
+      <c r="W26" s="22"/>
+      <c r="X26" s="14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>102</v>
       </c>
@@ -3115,38 +3209,43 @@
       <c r="G27" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="H27" s="24" t="s">
+      <c r="H27" s="14"/>
+      <c r="I27" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="J27" s="14"/>
+      <c r="K27" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="I27" s="24">
+      <c r="L27" s="24">
         <v>3</v>
       </c>
-      <c r="J27" s="57"/>
-      <c r="K27" s="57" t="s">
+      <c r="M27" s="57"/>
+      <c r="N27" s="57" t="s">
         <v>120</v>
       </c>
-      <c r="L27" s="25" t="s">
+      <c r="O27" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="M27" s="25"/>
-      <c r="N27" s="25" t="s">
+      <c r="P27" s="25"/>
+      <c r="Q27" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="O27" s="24" t="s">
+      <c r="R27" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="P27" s="24" t="s">
+      <c r="S27" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="Q27" s="14"/>
-      <c r="R27" s="14"/>
-      <c r="S27" s="26"/>
-      <c r="T27" s="22"/>
-      <c r="U27" s="14" t="s">
+      <c r="T27" s="14"/>
+      <c r="U27" s="14"/>
+      <c r="V27" s="26"/>
+      <c r="W27" s="22"/>
+      <c r="X27" s="14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>103</v>
       </c>
@@ -3160,38 +3259,43 @@
       <c r="G28" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="H28" s="27" t="s">
+      <c r="H28" s="14"/>
+      <c r="I28" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="J28" s="14"/>
+      <c r="K28" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="I28" s="27">
+      <c r="L28" s="27">
         <v>9</v>
       </c>
-      <c r="J28" s="57"/>
-      <c r="K28" s="57" t="s">
+      <c r="M28" s="57"/>
+      <c r="N28" s="57" t="s">
         <v>120</v>
       </c>
-      <c r="L28" s="27" t="s">
+      <c r="O28" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="M28" s="25"/>
-      <c r="N28" s="25" t="s">
+      <c r="P28" s="25"/>
+      <c r="Q28" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="O28" s="27" t="s">
+      <c r="R28" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="P28" s="25" t="s">
+      <c r="S28" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="Q28" s="14"/>
-      <c r="R28" s="14"/>
-      <c r="S28" s="26"/>
-      <c r="T28" s="22"/>
-      <c r="U28" s="14" t="s">
+      <c r="T28" s="14"/>
+      <c r="U28" s="14"/>
+      <c r="V28" s="26"/>
+      <c r="W28" s="22"/>
+      <c r="X28" s="14" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>104</v>
       </c>
@@ -3205,38 +3309,43 @@
       <c r="G29" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="H29" s="27" t="s">
+      <c r="H29" s="14"/>
+      <c r="I29" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="J29" s="14"/>
+      <c r="K29" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="I29" s="27">
+      <c r="L29" s="27">
         <v>9</v>
       </c>
-      <c r="J29" s="57"/>
-      <c r="K29" s="57" t="s">
+      <c r="M29" s="57"/>
+      <c r="N29" s="57" t="s">
         <v>120</v>
       </c>
-      <c r="L29" s="27" t="s">
+      <c r="O29" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="M29" s="25"/>
-      <c r="N29" s="25" t="s">
+      <c r="P29" s="25"/>
+      <c r="Q29" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="O29" s="27" t="s">
+      <c r="R29" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="P29" s="25" t="s">
+      <c r="S29" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="Q29" s="14"/>
-      <c r="R29" s="14"/>
-      <c r="S29" s="26"/>
-      <c r="T29" s="22"/>
-      <c r="U29" s="14" t="s">
+      <c r="T29" s="14"/>
+      <c r="U29" s="14"/>
+      <c r="V29" s="26"/>
+      <c r="W29" s="22"/>
+      <c r="X29" s="14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="28" t="s">
         <v>105</v>
       </c>
@@ -3250,38 +3359,43 @@
       <c r="G30" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="H30" s="29" t="s">
+      <c r="H30" s="28"/>
+      <c r="I30" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="J30" s="28"/>
+      <c r="K30" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="I30" s="29">
+      <c r="L30" s="29">
         <v>3</v>
       </c>
-      <c r="J30" s="58"/>
-      <c r="K30" s="58" t="s">
+      <c r="M30" s="58"/>
+      <c r="N30" s="58" t="s">
         <v>120</v>
       </c>
-      <c r="L30" s="30" t="s">
+      <c r="O30" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="M30" s="30"/>
-      <c r="N30" s="30" t="s">
+      <c r="P30" s="30"/>
+      <c r="Q30" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="O30" s="29" t="s">
+      <c r="R30" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="P30" s="29" t="s">
+      <c r="S30" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="Q30" s="28"/>
-      <c r="R30" s="28"/>
-      <c r="S30" s="31"/>
-      <c r="T30" s="22"/>
-      <c r="U30" s="14" t="s">
+      <c r="T30" s="28"/>
+      <c r="U30" s="28"/>
+      <c r="V30" s="31"/>
+      <c r="W30" s="22"/>
+      <c r="X30" s="14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="28" t="s">
         <v>106</v>
       </c>
@@ -3295,38 +3409,43 @@
       <c r="G31" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="H31" s="32" t="s">
+      <c r="H31" s="28"/>
+      <c r="I31" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="J31" s="28"/>
+      <c r="K31" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="I31" s="32">
+      <c r="L31" s="32">
         <v>9</v>
       </c>
-      <c r="J31" s="58"/>
-      <c r="K31" s="58" t="s">
+      <c r="M31" s="58"/>
+      <c r="N31" s="58" t="s">
         <v>120</v>
       </c>
-      <c r="L31" s="32" t="s">
+      <c r="O31" s="32" t="s">
         <v>123</v>
       </c>
-      <c r="M31" s="30"/>
-      <c r="N31" s="30" t="s">
+      <c r="P31" s="30"/>
+      <c r="Q31" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="O31" s="32" t="s">
+      <c r="R31" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="P31" s="30" t="s">
+      <c r="S31" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="Q31" s="28"/>
-      <c r="R31" s="28"/>
-      <c r="S31" s="31"/>
-      <c r="T31" s="22"/>
-      <c r="U31" s="14" t="s">
+      <c r="T31" s="28"/>
+      <c r="U31" s="28"/>
+      <c r="V31" s="31"/>
+      <c r="W31" s="22"/>
+      <c r="X31" s="14" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="36" t="s">
         <v>107</v>
       </c>
@@ -3344,24 +3463,27 @@
         <v>124</v>
       </c>
       <c r="G32" s="36"/>
-      <c r="H32" s="38"/>
-      <c r="I32" s="38"/>
-      <c r="J32" s="38"/>
+      <c r="H32" s="36"/>
+      <c r="I32" s="36"/>
+      <c r="J32" s="36"/>
       <c r="K32" s="38"/>
-      <c r="L32" s="43"/>
-      <c r="M32" s="39"/>
-      <c r="N32" s="39"/>
-      <c r="O32" s="38"/>
+      <c r="L32" s="38"/>
+      <c r="M32" s="38"/>
+      <c r="N32" s="38"/>
+      <c r="O32" s="43"/>
       <c r="P32" s="39"/>
-      <c r="Q32" s="36"/>
-      <c r="R32" s="36"/>
-      <c r="S32" s="40"/>
-      <c r="T32" s="41"/>
-      <c r="U32" s="33" t="s">
+      <c r="Q32" s="39"/>
+      <c r="R32" s="38"/>
+      <c r="S32" s="39"/>
+      <c r="T32" s="36"/>
+      <c r="U32" s="36"/>
+      <c r="V32" s="40"/>
+      <c r="W32" s="41"/>
+      <c r="X32" s="33" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33" s="36" t="s">
         <v>109</v>
       </c>
@@ -3371,42 +3493,31 @@
       <c r="C33" s="34"/>
       <c r="D33" s="34"/>
       <c r="E33" s="35"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="36" t="s">
-        <v>109</v>
-      </c>
-      <c r="H33" s="42" t="s">
-        <v>110</v>
-      </c>
-      <c r="I33" s="42">
-        <v>10</v>
-      </c>
-      <c r="J33" s="38"/>
-      <c r="K33" s="38" t="s">
-        <v>120</v>
-      </c>
-      <c r="L33" s="64" t="s">
-        <v>123</v>
-      </c>
-      <c r="M33" s="39"/>
-      <c r="N33" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="O33" s="42" t="s">
-        <v>110</v>
-      </c>
-      <c r="P33" s="43" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q33" s="36"/>
-      <c r="R33" s="36"/>
-      <c r="S33" s="40"/>
-      <c r="T33" s="41"/>
-      <c r="U33" s="33" t="s">
+      <c r="F33" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="G33" s="36"/>
+      <c r="H33" s="36"/>
+      <c r="I33" s="36"/>
+      <c r="J33" s="36"/>
+      <c r="K33" s="42"/>
+      <c r="L33" s="42"/>
+      <c r="M33" s="38"/>
+      <c r="N33" s="38"/>
+      <c r="O33" s="64"/>
+      <c r="P33" s="39"/>
+      <c r="Q33" s="39"/>
+      <c r="R33" s="42"/>
+      <c r="S33" s="43"/>
+      <c r="T33" s="36"/>
+      <c r="U33" s="36"/>
+      <c r="V33" s="40"/>
+      <c r="W33" s="41"/>
+      <c r="X33" s="33" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" s="44" t="s">
         <v>111</v>
       </c>
@@ -3420,38 +3531,43 @@
       <c r="G34" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="H34" s="45" t="s">
+      <c r="H34" s="44"/>
+      <c r="I34" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="J34" s="44"/>
+      <c r="K34" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="I34" s="45">
+      <c r="L34" s="45">
         <v>4</v>
       </c>
-      <c r="J34" s="45"/>
-      <c r="K34" s="45" t="s">
+      <c r="M34" s="45"/>
+      <c r="N34" s="45" t="s">
         <v>120</v>
       </c>
-      <c r="L34" s="49" t="s">
+      <c r="O34" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="M34" s="46"/>
-      <c r="N34" s="46" t="s">
+      <c r="P34" s="46"/>
+      <c r="Q34" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="O34" s="45" t="s">
+      <c r="R34" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="P34" s="46" t="s">
+      <c r="S34" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="Q34" s="44"/>
-      <c r="R34" s="44"/>
-      <c r="S34" s="47"/>
-      <c r="T34" s="41"/>
-      <c r="U34" s="33" t="s">
+      <c r="T34" s="44"/>
+      <c r="U34" s="44"/>
+      <c r="V34" s="47"/>
+      <c r="W34" s="41"/>
+      <c r="X34" s="33" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35" s="44" t="s">
         <v>112</v>
       </c>
@@ -3465,38 +3581,43 @@
       <c r="G35" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="H35" s="45" t="s">
+      <c r="H35" s="44"/>
+      <c r="I35" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="J35" s="44"/>
+      <c r="K35" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="I35" s="45">
+      <c r="L35" s="45">
         <v>4</v>
       </c>
-      <c r="J35" s="45"/>
-      <c r="K35" s="45" t="s">
+      <c r="M35" s="45"/>
+      <c r="N35" s="45" t="s">
         <v>120</v>
       </c>
-      <c r="L35" s="49" t="s">
+      <c r="O35" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="M35" s="46"/>
-      <c r="N35" s="46" t="s">
+      <c r="P35" s="46"/>
+      <c r="Q35" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="O35" s="45" t="s">
+      <c r="R35" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="P35" s="46" t="s">
+      <c r="S35" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="Q35" s="44"/>
-      <c r="R35" s="44"/>
-      <c r="S35" s="47"/>
-      <c r="T35" s="41"/>
-      <c r="U35" s="33" t="s">
+      <c r="T35" s="44"/>
+      <c r="U35" s="44"/>
+      <c r="V35" s="47"/>
+      <c r="W35" s="41"/>
+      <c r="X35" s="33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36" s="44" t="s">
         <v>113</v>
       </c>
@@ -3510,38 +3631,43 @@
       <c r="G36" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="H36" s="48" t="s">
+      <c r="H36" s="44"/>
+      <c r="I36" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="J36" s="44"/>
+      <c r="K36" s="48" t="s">
         <v>110</v>
       </c>
-      <c r="I36" s="48">
+      <c r="L36" s="48">
         <v>10</v>
       </c>
-      <c r="J36" s="45"/>
-      <c r="K36" s="45" t="s">
+      <c r="M36" s="45"/>
+      <c r="N36" s="45" t="s">
         <v>120</v>
       </c>
-      <c r="L36" s="65" t="s">
+      <c r="O36" s="65" t="s">
         <v>123</v>
       </c>
-      <c r="M36" s="46"/>
-      <c r="N36" s="46" t="s">
+      <c r="P36" s="46"/>
+      <c r="Q36" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="O36" s="48" t="s">
+      <c r="R36" s="48" t="s">
         <v>110</v>
       </c>
-      <c r="P36" s="49" t="s">
+      <c r="S36" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="Q36" s="44"/>
-      <c r="R36" s="44"/>
-      <c r="S36" s="47"/>
-      <c r="T36" s="41"/>
-      <c r="U36" s="33" t="s">
+      <c r="T36" s="44"/>
+      <c r="U36" s="44"/>
+      <c r="V36" s="47"/>
+      <c r="W36" s="41"/>
+      <c r="X36" s="33" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37" s="44" t="s">
         <v>114</v>
       </c>
@@ -3555,38 +3681,43 @@
       <c r="G37" s="44" t="s">
         <v>114</v>
       </c>
-      <c r="H37" s="45" t="s">
+      <c r="H37" s="44"/>
+      <c r="I37" s="44" t="s">
+        <v>114</v>
+      </c>
+      <c r="J37" s="44"/>
+      <c r="K37" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="I37" s="45">
+      <c r="L37" s="45">
         <v>4</v>
       </c>
-      <c r="J37" s="45"/>
-      <c r="K37" s="45" t="s">
+      <c r="M37" s="45"/>
+      <c r="N37" s="45" t="s">
         <v>120</v>
       </c>
-      <c r="L37" s="49" t="s">
+      <c r="O37" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="M37" s="46"/>
-      <c r="N37" s="46" t="s">
+      <c r="P37" s="46"/>
+      <c r="Q37" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="O37" s="45" t="s">
+      <c r="R37" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="P37" s="46" t="s">
+      <c r="S37" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="Q37" s="44"/>
-      <c r="R37" s="44"/>
-      <c r="S37" s="47"/>
-      <c r="T37" s="41"/>
-      <c r="U37" s="33" t="s">
+      <c r="T37" s="44"/>
+      <c r="U37" s="44"/>
+      <c r="V37" s="47"/>
+      <c r="W37" s="41"/>
+      <c r="X37" s="33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" s="44" t="s">
         <v>115</v>
       </c>
@@ -3600,38 +3731,43 @@
       <c r="G38" s="44" t="s">
         <v>115</v>
       </c>
-      <c r="H38" s="48" t="s">
+      <c r="H38" s="44"/>
+      <c r="I38" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="J38" s="44"/>
+      <c r="K38" s="48" t="s">
         <v>110</v>
       </c>
-      <c r="I38" s="48">
+      <c r="L38" s="48">
         <v>10</v>
       </c>
-      <c r="J38" s="45"/>
-      <c r="K38" s="45" t="s">
+      <c r="M38" s="45"/>
+      <c r="N38" s="45" t="s">
         <v>120</v>
       </c>
-      <c r="L38" s="65" t="s">
+      <c r="O38" s="65" t="s">
         <v>123</v>
       </c>
-      <c r="M38" s="46"/>
-      <c r="N38" s="46" t="s">
+      <c r="P38" s="46"/>
+      <c r="Q38" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="O38" s="48" t="s">
+      <c r="R38" s="48" t="s">
         <v>110</v>
       </c>
-      <c r="P38" s="49" t="s">
+      <c r="S38" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="Q38" s="44"/>
-      <c r="R38" s="44"/>
-      <c r="S38" s="47"/>
-      <c r="T38" s="41"/>
-      <c r="U38" s="33" t="s">
+      <c r="T38" s="44"/>
+      <c r="U38" s="44"/>
+      <c r="V38" s="47"/>
+      <c r="W38" s="41"/>
+      <c r="X38" s="33" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" s="44" t="s">
         <v>116</v>
       </c>
@@ -3645,38 +3781,43 @@
       <c r="G39" s="44" t="s">
         <v>116</v>
       </c>
-      <c r="H39" s="48" t="s">
+      <c r="H39" s="44"/>
+      <c r="I39" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="J39" s="44"/>
+      <c r="K39" s="48" t="s">
         <v>110</v>
       </c>
-      <c r="I39" s="48">
+      <c r="L39" s="48">
         <v>10</v>
       </c>
-      <c r="J39" s="45"/>
-      <c r="K39" s="45" t="s">
+      <c r="M39" s="45"/>
+      <c r="N39" s="45" t="s">
         <v>120</v>
       </c>
-      <c r="L39" s="65" t="s">
+      <c r="O39" s="65" t="s">
         <v>123</v>
       </c>
-      <c r="M39" s="46"/>
-      <c r="N39" s="46" t="s">
+      <c r="P39" s="46"/>
+      <c r="Q39" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="O39" s="48" t="s">
+      <c r="R39" s="48" t="s">
         <v>110</v>
       </c>
-      <c r="P39" s="49" t="s">
+      <c r="S39" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="Q39" s="44"/>
-      <c r="R39" s="44"/>
-      <c r="S39" s="47"/>
-      <c r="T39" s="41"/>
-      <c r="U39" s="33" t="s">
+      <c r="T39" s="44"/>
+      <c r="U39" s="44"/>
+      <c r="V39" s="47"/>
+      <c r="W39" s="41"/>
+      <c r="X39" s="33" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40" s="44" t="s">
         <v>117</v>
       </c>
@@ -3690,38 +3831,43 @@
       <c r="G40" s="44" t="s">
         <v>117</v>
       </c>
-      <c r="H40" s="45" t="s">
+      <c r="H40" s="44"/>
+      <c r="I40" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="J40" s="44"/>
+      <c r="K40" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="I40" s="45">
+      <c r="L40" s="45">
         <v>4</v>
       </c>
-      <c r="J40" s="45"/>
-      <c r="K40" s="45" t="s">
+      <c r="M40" s="45"/>
+      <c r="N40" s="45" t="s">
         <v>120</v>
       </c>
-      <c r="L40" s="49" t="s">
+      <c r="O40" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="M40" s="46"/>
-      <c r="N40" s="46" t="s">
+      <c r="P40" s="46"/>
+      <c r="Q40" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="O40" s="45" t="s">
+      <c r="R40" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="P40" s="46" t="s">
+      <c r="S40" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="Q40" s="44"/>
-      <c r="R40" s="44"/>
-      <c r="S40" s="47"/>
-      <c r="T40" s="41"/>
-      <c r="U40" s="33" t="s">
+      <c r="T40" s="44"/>
+      <c r="U40" s="44"/>
+      <c r="V40" s="47"/>
+      <c r="W40" s="41"/>
+      <c r="X40" s="33" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41" s="44" t="s">
         <v>118</v>
       </c>
@@ -3735,38 +3881,43 @@
       <c r="G41" s="44" t="s">
         <v>118</v>
       </c>
-      <c r="H41" s="48" t="s">
+      <c r="H41" s="44"/>
+      <c r="I41" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="J41" s="44"/>
+      <c r="K41" s="48" t="s">
         <v>110</v>
       </c>
-      <c r="I41" s="48">
+      <c r="L41" s="48">
         <v>10</v>
       </c>
-      <c r="J41" s="45"/>
-      <c r="K41" s="45" t="s">
+      <c r="M41" s="45"/>
+      <c r="N41" s="45" t="s">
         <v>120</v>
       </c>
-      <c r="L41" s="65" t="s">
+      <c r="O41" s="65" t="s">
         <v>123</v>
       </c>
-      <c r="M41" s="46"/>
-      <c r="N41" s="46" t="s">
+      <c r="P41" s="46"/>
+      <c r="Q41" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="O41" s="48" t="s">
+      <c r="R41" s="48" t="s">
         <v>110</v>
       </c>
-      <c r="P41" s="49" t="s">
+      <c r="S41" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="Q41" s="44"/>
-      <c r="R41" s="44"/>
-      <c r="S41" s="47"/>
-      <c r="T41" s="41"/>
-      <c r="U41" s="33" t="s">
+      <c r="T41" s="44"/>
+      <c r="U41" s="44"/>
+      <c r="V41" s="47"/>
+      <c r="W41" s="41"/>
+      <c r="X41" s="33" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
         <v>67</v>
       </c>
@@ -3784,24 +3935,27 @@
         <v>124</v>
       </c>
       <c r="G42" s="17"/>
-      <c r="H42" s="19"/>
-      <c r="I42" s="19"/>
-      <c r="J42" s="59"/>
-      <c r="K42" s="59"/>
-      <c r="L42" s="20"/>
-      <c r="M42" s="20"/>
-      <c r="N42" s="20"/>
-      <c r="O42" s="19"/>
-      <c r="P42" s="19"/>
-      <c r="Q42" s="17"/>
-      <c r="R42" s="17"/>
-      <c r="S42" s="21"/>
-      <c r="T42" s="22"/>
-      <c r="U42" s="14" t="s">
+      <c r="H42" s="17"/>
+      <c r="I42" s="17"/>
+      <c r="J42" s="17"/>
+      <c r="K42" s="19"/>
+      <c r="L42" s="19"/>
+      <c r="M42" s="59"/>
+      <c r="N42" s="59"/>
+      <c r="O42" s="20"/>
+      <c r="P42" s="20"/>
+      <c r="Q42" s="20"/>
+      <c r="R42" s="19"/>
+      <c r="S42" s="19"/>
+      <c r="T42" s="17"/>
+      <c r="U42" s="17"/>
+      <c r="V42" s="21"/>
+      <c r="W42" s="22"/>
+      <c r="X42" s="14" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
         <v>70</v>
       </c>
@@ -3811,42 +3965,31 @@
       <c r="C43" s="15"/>
       <c r="D43" s="15"/>
       <c r="E43" s="16"/>
-      <c r="F43" s="18"/>
-      <c r="G43" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="H43" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="I43" s="23">
-        <v>11</v>
-      </c>
-      <c r="J43" s="59"/>
-      <c r="K43" s="59" t="s">
-        <v>121</v>
-      </c>
-      <c r="L43" s="23" t="s">
-        <v>123</v>
-      </c>
-      <c r="M43" s="20"/>
-      <c r="N43" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="O43" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="P43" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q43" s="17"/>
-      <c r="R43" s="17"/>
-      <c r="S43" s="21"/>
-      <c r="T43" s="22"/>
-      <c r="U43" s="14" t="s">
+      <c r="F43" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="G43" s="17"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="17"/>
+      <c r="J43" s="17"/>
+      <c r="K43" s="23"/>
+      <c r="L43" s="23"/>
+      <c r="M43" s="59"/>
+      <c r="N43" s="59"/>
+      <c r="O43" s="23"/>
+      <c r="P43" s="20"/>
+      <c r="Q43" s="20"/>
+      <c r="R43" s="23"/>
+      <c r="S43" s="20"/>
+      <c r="T43" s="17"/>
+      <c r="U43" s="17"/>
+      <c r="V43" s="21"/>
+      <c r="W43" s="22"/>
+      <c r="X43" s="14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
         <v>73</v>
       </c>
@@ -3860,38 +4003,43 @@
       <c r="G44" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="H44" s="24" t="s">
+      <c r="H44" s="14"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="K44" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="I44" s="24">
+      <c r="L44" s="24">
         <v>5</v>
       </c>
-      <c r="J44" s="60"/>
-      <c r="K44" s="60" t="s">
+      <c r="M44" s="60"/>
+      <c r="N44" s="60" t="s">
         <v>121</v>
       </c>
-      <c r="L44" s="25" t="s">
+      <c r="O44" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="M44" s="25"/>
-      <c r="N44" s="25" t="s">
+      <c r="P44" s="25"/>
+      <c r="Q44" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="O44" s="24" t="s">
+      <c r="R44" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="P44" s="24" t="s">
+      <c r="S44" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="Q44" s="14"/>
-      <c r="R44" s="14"/>
-      <c r="S44" s="26"/>
-      <c r="T44" s="22"/>
-      <c r="U44" s="14" t="s">
+      <c r="T44" s="14"/>
+      <c r="U44" s="14"/>
+      <c r="V44" s="26"/>
+      <c r="W44" s="22"/>
+      <c r="X44" s="14" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
         <v>74</v>
       </c>
@@ -3905,38 +4053,43 @@
       <c r="G45" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="H45" s="24" t="s">
+      <c r="H45" s="14"/>
+      <c r="I45" s="14"/>
+      <c r="J45" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="K45" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="I45" s="24">
+      <c r="L45" s="24">
         <v>5</v>
       </c>
-      <c r="J45" s="60"/>
-      <c r="K45" s="60" t="s">
+      <c r="M45" s="60"/>
+      <c r="N45" s="60" t="s">
         <v>121</v>
       </c>
-      <c r="L45" s="25" t="s">
+      <c r="O45" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="M45" s="25"/>
-      <c r="N45" s="25" t="s">
+      <c r="P45" s="25"/>
+      <c r="Q45" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="O45" s="24" t="s">
+      <c r="R45" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="P45" s="24" t="s">
+      <c r="S45" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="Q45" s="14"/>
-      <c r="R45" s="14"/>
-      <c r="S45" s="26"/>
-      <c r="T45" s="22"/>
-      <c r="U45" s="14" t="s">
+      <c r="T45" s="14"/>
+      <c r="U45" s="14"/>
+      <c r="V45" s="26"/>
+      <c r="W45" s="22"/>
+      <c r="X45" s="14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46" s="14" t="s">
         <v>75</v>
       </c>
@@ -3950,38 +4103,43 @@
       <c r="G46" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="H46" s="27" t="s">
+      <c r="H46" s="14"/>
+      <c r="I46" s="14"/>
+      <c r="J46" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="K46" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="I46" s="27">
+      <c r="L46" s="27">
         <v>11</v>
       </c>
-      <c r="J46" s="60"/>
-      <c r="K46" s="60" t="s">
+      <c r="M46" s="60"/>
+      <c r="N46" s="60" t="s">
         <v>121</v>
       </c>
-      <c r="L46" s="27" t="s">
+      <c r="O46" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="M46" s="25"/>
-      <c r="N46" s="25" t="s">
+      <c r="P46" s="25"/>
+      <c r="Q46" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="O46" s="27" t="s">
+      <c r="R46" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="P46" s="25" t="s">
+      <c r="S46" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="Q46" s="14"/>
-      <c r="R46" s="14"/>
-      <c r="S46" s="26"/>
-      <c r="T46" s="22"/>
-      <c r="U46" s="14" t="s">
+      <c r="T46" s="14"/>
+      <c r="U46" s="14"/>
+      <c r="V46" s="26"/>
+      <c r="W46" s="22"/>
+      <c r="X46" s="14" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
         <v>76</v>
       </c>
@@ -3995,38 +4153,43 @@
       <c r="G47" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="H47" s="24" t="s">
+      <c r="H47" s="14"/>
+      <c r="I47" s="14"/>
+      <c r="J47" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="K47" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="I47" s="24">
+      <c r="L47" s="24">
         <v>5</v>
       </c>
-      <c r="J47" s="60"/>
-      <c r="K47" s="60" t="s">
+      <c r="M47" s="60"/>
+      <c r="N47" s="60" t="s">
         <v>121</v>
       </c>
-      <c r="L47" s="25" t="s">
+      <c r="O47" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="M47" s="25"/>
-      <c r="N47" s="25" t="s">
+      <c r="P47" s="25"/>
+      <c r="Q47" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="O47" s="24" t="s">
+      <c r="R47" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="P47" s="24" t="s">
+      <c r="S47" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="Q47" s="14"/>
-      <c r="R47" s="14"/>
-      <c r="S47" s="26"/>
-      <c r="T47" s="22"/>
-      <c r="U47" s="14" t="s">
+      <c r="T47" s="14"/>
+      <c r="U47" s="14"/>
+      <c r="V47" s="26"/>
+      <c r="W47" s="22"/>
+      <c r="X47" s="14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
         <v>77</v>
       </c>
@@ -4040,38 +4203,43 @@
       <c r="G48" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="H48" s="27" t="s">
+      <c r="H48" s="14"/>
+      <c r="I48" s="14"/>
+      <c r="J48" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="K48" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="I48" s="27">
+      <c r="L48" s="27">
         <v>11</v>
       </c>
-      <c r="J48" s="60"/>
-      <c r="K48" s="60" t="s">
+      <c r="M48" s="60"/>
+      <c r="N48" s="60" t="s">
         <v>121</v>
       </c>
-      <c r="L48" s="27" t="s">
+      <c r="O48" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="M48" s="25"/>
-      <c r="N48" s="25" t="s">
+      <c r="P48" s="25"/>
+      <c r="Q48" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="O48" s="27" t="s">
+      <c r="R48" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="P48" s="25" t="s">
+      <c r="S48" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="Q48" s="14"/>
-      <c r="R48" s="14"/>
-      <c r="S48" s="26"/>
-      <c r="T48" s="22"/>
-      <c r="U48" s="14" t="s">
+      <c r="T48" s="14"/>
+      <c r="U48" s="14"/>
+      <c r="V48" s="26"/>
+      <c r="W48" s="22"/>
+      <c r="X48" s="14" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
         <v>78</v>
       </c>
@@ -4085,38 +4253,43 @@
       <c r="G49" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="H49" s="27" t="s">
+      <c r="H49" s="14"/>
+      <c r="I49" s="14"/>
+      <c r="J49" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="K49" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="I49" s="27">
+      <c r="L49" s="27">
         <v>11</v>
       </c>
-      <c r="J49" s="60"/>
-      <c r="K49" s="60" t="s">
+      <c r="M49" s="60"/>
+      <c r="N49" s="60" t="s">
         <v>121</v>
       </c>
-      <c r="L49" s="27" t="s">
+      <c r="O49" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="M49" s="25"/>
-      <c r="N49" s="25" t="s">
+      <c r="P49" s="25"/>
+      <c r="Q49" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="O49" s="27" t="s">
+      <c r="R49" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="P49" s="25" t="s">
+      <c r="S49" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="Q49" s="14"/>
-      <c r="R49" s="14"/>
-      <c r="S49" s="26"/>
-      <c r="T49" s="22"/>
-      <c r="U49" s="14" t="s">
+      <c r="T49" s="14"/>
+      <c r="U49" s="14"/>
+      <c r="V49" s="26"/>
+      <c r="W49" s="22"/>
+      <c r="X49" s="14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50" s="28" t="s">
         <v>79</v>
       </c>
@@ -4130,38 +4303,43 @@
       <c r="G50" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="H50" s="29" t="s">
+      <c r="H50" s="28"/>
+      <c r="I50" s="28"/>
+      <c r="J50" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="K50" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="I50" s="29">
+      <c r="L50" s="29">
         <v>5</v>
       </c>
-      <c r="J50" s="61"/>
-      <c r="K50" s="61" t="s">
+      <c r="M50" s="61"/>
+      <c r="N50" s="61" t="s">
         <v>121</v>
       </c>
-      <c r="L50" s="30" t="s">
+      <c r="O50" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="M50" s="30"/>
-      <c r="N50" s="30" t="s">
+      <c r="P50" s="30"/>
+      <c r="Q50" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="O50" s="29" t="s">
+      <c r="R50" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="P50" s="29" t="s">
+      <c r="S50" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="Q50" s="28"/>
-      <c r="R50" s="28"/>
-      <c r="S50" s="31"/>
-      <c r="T50" s="22"/>
-      <c r="U50" s="14" t="s">
+      <c r="T50" s="28"/>
+      <c r="U50" s="28"/>
+      <c r="V50" s="31"/>
+      <c r="W50" s="22"/>
+      <c r="X50" s="14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51" s="28" t="s">
         <v>80</v>
       </c>
@@ -4175,38 +4353,43 @@
       <c r="G51" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="H51" s="32" t="s">
+      <c r="H51" s="28"/>
+      <c r="I51" s="28"/>
+      <c r="J51" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="K51" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="I51" s="32">
+      <c r="L51" s="32">
         <v>11</v>
       </c>
-      <c r="J51" s="61"/>
-      <c r="K51" s="61" t="s">
+      <c r="M51" s="61"/>
+      <c r="N51" s="61" t="s">
         <v>121</v>
       </c>
-      <c r="L51" s="32" t="s">
+      <c r="O51" s="32" t="s">
         <v>123</v>
       </c>
-      <c r="M51" s="30"/>
-      <c r="N51" s="30" t="s">
+      <c r="P51" s="30"/>
+      <c r="Q51" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="O51" s="32" t="s">
+      <c r="R51" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="P51" s="30" t="s">
+      <c r="S51" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="Q51" s="28"/>
-      <c r="R51" s="28"/>
-      <c r="S51" s="31"/>
-      <c r="T51" s="22"/>
-      <c r="U51" s="14" t="s">
+      <c r="T51" s="28"/>
+      <c r="U51" s="28"/>
+      <c r="V51" s="31"/>
+      <c r="W51" s="22"/>
+      <c r="X51" s="14" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52" s="36" t="s">
         <v>81</v>
       </c>
@@ -4224,24 +4407,27 @@
         <v>124</v>
       </c>
       <c r="G52" s="36"/>
-      <c r="H52" s="38"/>
-      <c r="I52" s="38"/>
-      <c r="J52" s="62"/>
-      <c r="K52" s="62"/>
-      <c r="L52" s="43"/>
-      <c r="M52" s="39"/>
-      <c r="N52" s="39"/>
-      <c r="O52" s="38"/>
+      <c r="H52" s="36"/>
+      <c r="I52" s="36"/>
+      <c r="J52" s="36"/>
+      <c r="K52" s="38"/>
+      <c r="L52" s="38"/>
+      <c r="M52" s="62"/>
+      <c r="N52" s="62"/>
+      <c r="O52" s="43"/>
       <c r="P52" s="39"/>
-      <c r="Q52" s="36"/>
-      <c r="R52" s="36"/>
-      <c r="S52" s="40"/>
-      <c r="T52" s="41"/>
-      <c r="U52" s="33" t="s">
+      <c r="Q52" s="39"/>
+      <c r="R52" s="38"/>
+      <c r="S52" s="39"/>
+      <c r="T52" s="36"/>
+      <c r="U52" s="36"/>
+      <c r="V52" s="40"/>
+      <c r="W52" s="41"/>
+      <c r="X52" s="33" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53" s="36" t="s">
         <v>83</v>
       </c>
@@ -4251,42 +4437,31 @@
       <c r="C53" s="34"/>
       <c r="D53" s="34"/>
       <c r="E53" s="35"/>
-      <c r="F53" s="37"/>
-      <c r="G53" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="H53" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="I53" s="42">
-        <v>12</v>
-      </c>
-      <c r="J53" s="62"/>
-      <c r="K53" s="62" t="s">
-        <v>121</v>
-      </c>
-      <c r="L53" s="64" t="s">
-        <v>123</v>
-      </c>
-      <c r="M53" s="39"/>
-      <c r="N53" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="O53" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="P53" s="43" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q53" s="36"/>
-      <c r="R53" s="36"/>
-      <c r="S53" s="40"/>
-      <c r="T53" s="41"/>
-      <c r="U53" s="33" t="s">
+      <c r="F53" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="G53" s="36"/>
+      <c r="H53" s="36"/>
+      <c r="I53" s="36"/>
+      <c r="J53" s="36"/>
+      <c r="K53" s="42"/>
+      <c r="L53" s="42"/>
+      <c r="M53" s="62"/>
+      <c r="N53" s="62"/>
+      <c r="O53" s="64"/>
+      <c r="P53" s="39"/>
+      <c r="Q53" s="39"/>
+      <c r="R53" s="42"/>
+      <c r="S53" s="43"/>
+      <c r="T53" s="36"/>
+      <c r="U53" s="36"/>
+      <c r="V53" s="40"/>
+      <c r="W53" s="41"/>
+      <c r="X53" s="33" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54" s="44" t="s">
         <v>85</v>
       </c>
@@ -4300,38 +4475,43 @@
       <c r="G54" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="H54" s="45" t="s">
+      <c r="H54" s="44"/>
+      <c r="I54" s="44"/>
+      <c r="J54" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="K54" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="I54" s="45">
+      <c r="L54" s="45">
         <v>6</v>
       </c>
-      <c r="J54" s="63"/>
-      <c r="K54" s="63" t="s">
+      <c r="M54" s="63"/>
+      <c r="N54" s="63" t="s">
         <v>121</v>
       </c>
-      <c r="L54" s="49" t="s">
+      <c r="O54" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="M54" s="46"/>
-      <c r="N54" s="46" t="s">
+      <c r="P54" s="46"/>
+      <c r="Q54" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="O54" s="45" t="s">
+      <c r="R54" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="P54" s="46" t="s">
+      <c r="S54" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="Q54" s="44"/>
-      <c r="R54" s="44"/>
-      <c r="S54" s="47"/>
-      <c r="T54" s="41"/>
-      <c r="U54" s="33" t="s">
+      <c r="T54" s="44"/>
+      <c r="U54" s="44"/>
+      <c r="V54" s="47"/>
+      <c r="W54" s="41"/>
+      <c r="X54" s="33" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55" s="44" t="s">
         <v>86</v>
       </c>
@@ -4345,38 +4525,43 @@
       <c r="G55" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="H55" s="45" t="s">
+      <c r="H55" s="44"/>
+      <c r="I55" s="44"/>
+      <c r="J55" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="K55" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="I55" s="45">
+      <c r="L55" s="45">
         <v>6</v>
       </c>
-      <c r="J55" s="63"/>
-      <c r="K55" s="63" t="s">
+      <c r="M55" s="63"/>
+      <c r="N55" s="63" t="s">
         <v>121</v>
       </c>
-      <c r="L55" s="49" t="s">
+      <c r="O55" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="M55" s="46"/>
-      <c r="N55" s="46" t="s">
+      <c r="P55" s="46"/>
+      <c r="Q55" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="O55" s="45" t="s">
+      <c r="R55" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="P55" s="46" t="s">
+      <c r="S55" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="Q55" s="44"/>
-      <c r="R55" s="44"/>
-      <c r="S55" s="47"/>
-      <c r="T55" s="41"/>
-      <c r="U55" s="33" t="s">
+      <c r="T55" s="44"/>
+      <c r="U55" s="44"/>
+      <c r="V55" s="47"/>
+      <c r="W55" s="41"/>
+      <c r="X55" s="33" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A56" s="44" t="s">
         <v>87</v>
       </c>
@@ -4390,38 +4575,43 @@
       <c r="G56" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="H56" s="48" t="s">
+      <c r="H56" s="44"/>
+      <c r="I56" s="44"/>
+      <c r="J56" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="K56" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="I56" s="48">
+      <c r="L56" s="48">
         <v>12</v>
       </c>
-      <c r="J56" s="63"/>
-      <c r="K56" s="63" t="s">
+      <c r="M56" s="63"/>
+      <c r="N56" s="63" t="s">
         <v>121</v>
       </c>
-      <c r="L56" s="65" t="s">
+      <c r="O56" s="65" t="s">
         <v>123</v>
       </c>
-      <c r="M56" s="46"/>
-      <c r="N56" s="46" t="s">
+      <c r="P56" s="46"/>
+      <c r="Q56" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="O56" s="48" t="s">
+      <c r="R56" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="P56" s="49" t="s">
+      <c r="S56" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="Q56" s="44"/>
-      <c r="R56" s="44"/>
-      <c r="S56" s="47"/>
-      <c r="T56" s="41"/>
-      <c r="U56" s="33" t="s">
+      <c r="T56" s="44"/>
+      <c r="U56" s="44"/>
+      <c r="V56" s="47"/>
+      <c r="W56" s="41"/>
+      <c r="X56" s="33" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A57" s="44" t="s">
         <v>88</v>
       </c>
@@ -4435,38 +4625,43 @@
       <c r="G57" s="44" t="s">
         <v>88</v>
       </c>
-      <c r="H57" s="45" t="s">
+      <c r="H57" s="44"/>
+      <c r="I57" s="44"/>
+      <c r="J57" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="K57" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="I57" s="45">
+      <c r="L57" s="45">
         <v>6</v>
       </c>
-      <c r="J57" s="63"/>
-      <c r="K57" s="63" t="s">
+      <c r="M57" s="63"/>
+      <c r="N57" s="63" t="s">
         <v>121</v>
       </c>
-      <c r="L57" s="49" t="s">
+      <c r="O57" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="M57" s="46"/>
-      <c r="N57" s="46" t="s">
+      <c r="P57" s="46"/>
+      <c r="Q57" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="O57" s="45" t="s">
+      <c r="R57" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="P57" s="46" t="s">
+      <c r="S57" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="Q57" s="44"/>
-      <c r="R57" s="44"/>
-      <c r="S57" s="47"/>
-      <c r="T57" s="41"/>
-      <c r="U57" s="33" t="s">
+      <c r="T57" s="44"/>
+      <c r="U57" s="44"/>
+      <c r="V57" s="47"/>
+      <c r="W57" s="41"/>
+      <c r="X57" s="33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58" s="44" t="s">
         <v>89</v>
       </c>
@@ -4480,38 +4675,43 @@
       <c r="G58" s="44" t="s">
         <v>89</v>
       </c>
-      <c r="H58" s="48" t="s">
+      <c r="H58" s="44"/>
+      <c r="I58" s="44"/>
+      <c r="J58" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="K58" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="I58" s="48">
+      <c r="L58" s="48">
         <v>12</v>
       </c>
-      <c r="J58" s="63"/>
-      <c r="K58" s="63" t="s">
+      <c r="M58" s="63"/>
+      <c r="N58" s="63" t="s">
         <v>121</v>
       </c>
-      <c r="L58" s="65" t="s">
+      <c r="O58" s="65" t="s">
         <v>123</v>
       </c>
-      <c r="M58" s="46"/>
-      <c r="N58" s="46" t="s">
+      <c r="P58" s="46"/>
+      <c r="Q58" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="O58" s="48" t="s">
+      <c r="R58" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="P58" s="49" t="s">
+      <c r="S58" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="Q58" s="44"/>
-      <c r="R58" s="44"/>
-      <c r="S58" s="47"/>
-      <c r="T58" s="41"/>
-      <c r="U58" s="33" t="s">
+      <c r="T58" s="44"/>
+      <c r="U58" s="44"/>
+      <c r="V58" s="47"/>
+      <c r="W58" s="41"/>
+      <c r="X58" s="33" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A59" s="44" t="s">
         <v>90</v>
       </c>
@@ -4525,38 +4725,43 @@
       <c r="G59" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="H59" s="48" t="s">
+      <c r="H59" s="44"/>
+      <c r="I59" s="44"/>
+      <c r="J59" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="K59" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="I59" s="48">
+      <c r="L59" s="48">
         <v>12</v>
       </c>
-      <c r="J59" s="63"/>
-      <c r="K59" s="63" t="s">
+      <c r="M59" s="63"/>
+      <c r="N59" s="63" t="s">
         <v>121</v>
       </c>
-      <c r="L59" s="65" t="s">
+      <c r="O59" s="65" t="s">
         <v>123</v>
       </c>
-      <c r="M59" s="46"/>
-      <c r="N59" s="46" t="s">
+      <c r="P59" s="46"/>
+      <c r="Q59" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="O59" s="48" t="s">
+      <c r="R59" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="P59" s="49" t="s">
+      <c r="S59" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="Q59" s="44"/>
-      <c r="R59" s="44"/>
-      <c r="S59" s="47"/>
-      <c r="T59" s="41"/>
-      <c r="U59" s="33" t="s">
+      <c r="T59" s="44"/>
+      <c r="U59" s="44"/>
+      <c r="V59" s="47"/>
+      <c r="W59" s="41"/>
+      <c r="X59" s="33" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60" s="44" t="s">
         <v>91</v>
       </c>
@@ -4570,38 +4775,43 @@
       <c r="G60" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="H60" s="45" t="s">
+      <c r="H60" s="44"/>
+      <c r="I60" s="44"/>
+      <c r="J60" s="44" t="s">
+        <v>91</v>
+      </c>
+      <c r="K60" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="I60" s="45">
+      <c r="L60" s="45">
         <v>6</v>
       </c>
-      <c r="J60" s="63"/>
-      <c r="K60" s="63" t="s">
+      <c r="M60" s="63"/>
+      <c r="N60" s="63" t="s">
         <v>121</v>
       </c>
-      <c r="L60" s="49" t="s">
+      <c r="O60" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="M60" s="46"/>
-      <c r="N60" s="46" t="s">
+      <c r="P60" s="46"/>
+      <c r="Q60" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="O60" s="45" t="s">
+      <c r="R60" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="P60" s="46" t="s">
+      <c r="S60" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="Q60" s="44"/>
-      <c r="R60" s="44"/>
-      <c r="S60" s="47"/>
-      <c r="T60" s="41"/>
-      <c r="U60" s="33" t="s">
+      <c r="T60" s="44"/>
+      <c r="U60" s="44"/>
+      <c r="V60" s="47"/>
+      <c r="W60" s="41"/>
+      <c r="X60" s="33" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A61" s="44" t="s">
         <v>92</v>
       </c>
@@ -4615,34 +4825,39 @@
       <c r="G61" s="44" t="s">
         <v>92</v>
       </c>
-      <c r="H61" s="48" t="s">
+      <c r="H61" s="44"/>
+      <c r="I61" s="44"/>
+      <c r="J61" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="K61" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="I61" s="48">
+      <c r="L61" s="48">
         <v>12</v>
       </c>
-      <c r="J61" s="63"/>
-      <c r="K61" s="63" t="s">
+      <c r="M61" s="63"/>
+      <c r="N61" s="63" t="s">
         <v>121</v>
       </c>
-      <c r="L61" s="65" t="s">
+      <c r="O61" s="65" t="s">
         <v>123</v>
       </c>
-      <c r="M61" s="46"/>
-      <c r="N61" s="46" t="s">
+      <c r="P61" s="46"/>
+      <c r="Q61" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="O61" s="48" t="s">
+      <c r="R61" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="P61" s="49" t="s">
+      <c r="S61" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="Q61" s="44"/>
-      <c r="R61" s="44"/>
-      <c r="S61" s="47"/>
-      <c r="T61" s="41"/>
-      <c r="U61" s="33" t="s">
+      <c r="T61" s="44"/>
+      <c r="U61" s="44"/>
+      <c r="V61" s="47"/>
+      <c r="W61" s="41"/>
+      <c r="X61" s="33" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update notes to column keys in metadata files (Excel)
</commit_message>
<xml_diff>
--- a/inst/extdata/expt_smry_cptac_cmbn.xlsx
+++ b/inst/extdata/expt_smry_cptac_cmbn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Results\R\proteoQDA\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C362217B-950E-4B15-B785-2F97B4BE7869}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7C0F96-5F51-42CA-844D-D5986EC4FE8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20700" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
     <author>Qiang Zhang</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{B80D651D-92A1-4F53-814E-F096240C02BD}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{91D0C885-3698-421C-AE62-CFFAD7A9E118}">
       <text>
         <r>
           <rPr>
@@ -44,20 +44,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> sample IDs</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{6B225692-AE40-4A9C-94D8-4974D8522A4F}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Enter "?setup_expts" under an </t>
+          <t xml:space="preserve"> sample IDs 
+(Enter "?setup_expts" under an </t>
         </r>
         <r>
           <rPr>
@@ -76,31 +64,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> console for details of the column keys.
-Column keys </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>A1 - H1</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> are reserved.</t>
+          <t xml:space="preserve"> console for details of the column keys.)</t>
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{6B4E9D35-A084-43B7-8521-08976BB66C1A}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{312F59BA-722C-4C53-BD4D-048705CB28BF}">
       <text>
         <r>
           <rPr>
@@ -109,7 +77,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">The file names of RAW MS data. Use file </t>
+          <t xml:space="preserve">The file names of RAW MS data
+(Enter alternatively the file names in </t>
         </r>
         <r>
           <rPr>
@@ -128,11 +97,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> if more than one RAW file per TMT set</t>
+          <t xml:space="preserve"> if more than one RAW file per TMT set)</t>
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{20ED1DA0-9072-4294-9742-D28F4D21C286}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{E7609BE5-6D37-4CCF-9C1A-DE8F1D1C7320}">
       <text>
         <r>
           <rPr>
@@ -141,11 +110,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Sample IDs being references</t>
+          <t>Non-void character strings to indicate refernce channels.</t>
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{C7838A55-CA27-4058-92FF-4A89D46A1BEE}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{B6CEE270-8CBF-47E9-A853-074E59253477}">
       <text>
         <r>
           <rPr>
@@ -154,7 +123,27 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Samples will be included in analysis</t>
+          <t xml:space="preserve">Samples to be selected for analyses 
+(Enter "?setup_expts" under an </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>R</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> console for details of the column keys.)</t>
         </r>
       </text>
     </comment>
@@ -1395,7 +1384,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1432,6 +1421,9 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1767,10 +1759,20 @@
   <dimension ref="A1:AH61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AH1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
@@ -1779,10 +1781,10 @@
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="13" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="2" t="s">

</xml_diff>

<commit_message>
Update notes to metadata column keys
</commit_message>
<xml_diff>
--- a/inst/extdata/expt_smry_cptac_cmbn.xlsx
+++ b/inst/extdata/expt_smry_cptac_cmbn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Results\R\proteoQDA\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7C0F96-5F51-42CA-844D-D5986EC4FE8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CDF0E1-4D34-472A-A1EC-C1A39A2A7431}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20700" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve"> sample IDs 
-(Enter "?setup_expts" under an </t>
+(Enter "?load_expts" under an </t>
         </r>
         <r>
           <rPr>
@@ -124,7 +124,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">Samples to be selected for analyses 
-(Enter "?setup_expts" under an </t>
+(Enter "?load_expts" under an </t>
         </r>
         <r>
           <rPr>
@@ -1759,7 +1759,7 @@
   <dimension ref="A1:AH61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>